<commit_message>
solved environment problem, next up is erosion blocks
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43AA399F-2385-4385-84CC-BBA8134E21D9}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6608922-8D71-43D0-A36E-0B61F1614210}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="171">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -536,13 +536,22 @@
   </si>
   <si>
     <t>The hotstart problem was in the python toolbox, where hotstart is not yet added as a possible variable in the set_params function. The hotstart does seem to be working now.</t>
+  </si>
+  <si>
+    <t>We see slumping and delayed freezup as a result from the increased node threshold. I also see that the October storm does not really affect the coast because of the timing being just after freeze-up! I do see some weird behaviour where enthalpy dispersal seems lower for some of the models, especially when the entire thing is around melting temperature.</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>Has all newest functionality (increased node threshold, hotstart), but used to test era5 data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +682,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1073,7 +1088,6 @@
   <dxfs count="14">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1098,6 +1112,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1162,16 +1177,16 @@
     <tableColumn id="2" xr3:uid="{4CCC7AF7-3469-4B96-A652-EA36B38CE976}" uniqueName="2" name="t_start" queryTableFieldId="2" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{46F8B739-DA88-47AA-AFA1-33CDA573621E}" uniqueName="3" name="t_end" queryTableFieldId="3" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{7E93C469-DCA2-46FF-9D96-8A54E5DA317D}" uniqueName="4" name="description" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{1CEA6FCD-46CD-47DB-BA27-194DF50C2DF3}" uniqueName="5" name="Column1" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{96686839-3084-4A1F-856F-D4361C25D5FA}" uniqueName="6" name="_1" queryTableFieldId="6" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{4081C439-4753-405E-AF0D-2B097433B57E}" uniqueName="7" name="_2" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{DF7FDA72-7DCE-410C-A691-A70C7F3278D3}" uniqueName="8" name="_3" queryTableFieldId="8" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{3E902B63-1F9F-41E2-A4BF-60D0E33B320C}" uniqueName="9" name="_4" queryTableFieldId="9" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{47AD3BB5-933D-4516-9CE8-D2DF8E8484A3}" uniqueName="10" name="_5" queryTableFieldId="10" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{DCA43BF2-2100-4DA2-A135-03D3E51FAD07}" uniqueName="11" name="_6" queryTableFieldId="11" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{6A4AFB09-1817-4575-BB30-DF8C1B5156B2}" uniqueName="12" name="_7" queryTableFieldId="12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{96860A53-4017-4086-81CB-1927DFFA9764}" uniqueName="13" name="_8" queryTableFieldId="13" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{438B3ECA-A5E6-4FE9-890C-0D6216396AFC}" uniqueName="14" name="_9" queryTableFieldId="14" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1CEA6FCD-46CD-47DB-BA27-194DF50C2DF3}" uniqueName="5" name="Column1" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{96686839-3084-4A1F-856F-D4361C25D5FA}" uniqueName="6" name="_1" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4081C439-4753-405E-AF0D-2B097433B57E}" uniqueName="7" name="_2" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{DF7FDA72-7DCE-410C-A691-A70C7F3278D3}" uniqueName="8" name="_3" queryTableFieldId="8" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{3E902B63-1F9F-41E2-A4BF-60D0E33B320C}" uniqueName="9" name="_4" queryTableFieldId="9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{47AD3BB5-933D-4516-9CE8-D2DF8E8484A3}" uniqueName="10" name="_5" queryTableFieldId="10" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{DCA43BF2-2100-4DA2-A135-03D3E51FAD07}" uniqueName="11" name="_6" queryTableFieldId="11" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{6A4AFB09-1817-4575-BB30-DF8C1B5156B2}" uniqueName="12" name="_7" queryTableFieldId="12" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{96860A53-4017-4086-81CB-1927DFFA9764}" uniqueName="13" name="_8" queryTableFieldId="13" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{438B3ECA-A5E6-4FE9-890C-0D6216396AFC}" uniqueName="14" name="_9" queryTableFieldId="14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1496,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D62850-41A0-483E-B58F-AB9686CF6265}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2383,7 +2398,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>163</v>
       </c>
@@ -2400,7 +2415,7 @@
         <v>79</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>79</v>
+        <v>168</v>
       </c>
       <c r="G21" t="s">
         <v>79</v>
@@ -2473,12 +2488,16 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40806</v>
+      </c>
+      <c r="C23" s="1">
+        <v>40817</v>
+      </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
         <v>79</v>
@@ -4124,6 +4143,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
inclusion of water level data, generation of new storm.csv finalized, setup of test run
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B646A81-BCFD-450B-AD47-C634A6A471F0}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAD9357-FF55-4C1E-B2F1-9289BEFAF05F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="175">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -550,7 +550,13 @@
     <t>val8_xb</t>
   </si>
   <si>
-    <t>Same as val7_xb, but with skewness/asymmetry/… factor set to 0, to try to reduce onshore transport</t>
+    <t>test_xb</t>
+  </si>
+  <si>
+    <t>Same as val8_xb, but shorter to test era5 storm data with Kees' water levels. Also included the new water level data in other parts of the model, such as the temperature computation. Also has higher friction value (0.02 instead of 0.01). Have not yet increased the critical bluff slope</t>
+  </si>
+  <si>
+    <t>Same as val7_xb, but with skewness/asymmetry/… factor set to 0, to try to reduce onshore transport. Also removed viscosity specification.</t>
   </si>
 </sst>
 </file>
@@ -2547,7 +2553,7 @@
         <v>44561</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
         <v>79</v>
@@ -2582,12 +2588,16 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="B25" s="1">
+        <v>40806</v>
+      </c>
+      <c r="C25" s="1">
+        <v>40817</v>
+      </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="E25" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
computed critical slopes from data, added interpretation of val8_xb, and setup for run val9_xb
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAD9357-FF55-4C1E-B2F1-9289BEFAF05F}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77891D8F-AAED-4ACF-B048-30D5C9C464FE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="179">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -550,13 +550,25 @@
     <t>val8_xb</t>
   </si>
   <si>
-    <t>test_xb</t>
-  </si>
-  <si>
     <t>Same as val8_xb, but shorter to test era5 storm data with Kees' water levels. Also included the new water level data in other parts of the model, such as the temperature computation. Also has higher friction value (0.02 instead of 0.01). Have not yet increased the critical bluff slope</t>
   </si>
   <si>
     <t>Same as val7_xb, but with skewness/asymmetry/… factor set to 0, to try to reduce onshore transport. Also removed viscosity specification.</t>
+  </si>
+  <si>
+    <t>val9_xb</t>
+  </si>
+  <si>
+    <t>test6 (re-run)</t>
+  </si>
+  <si>
+    <t>Increased wet &amp; dry slope, increased modelling depth</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>We see slumping followed by offshore transport!!! The offshore transport is currently strong enough to actually carry the material away from the bluff toe, and we see significant bluff retreat after 1 year. What's also interesting, is that for 2021, there are hardly any significant storms until well into september. The thawed material stays on the bluff, and insulates the deeper material. When a storm finally hits and transports the material offshore, it's too late into the season to see significant slumping. This leads to very little erosion that year.</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1058,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1523,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D62850-41A0-483E-B58F-AB9686CF6265}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2514,8 +2529,8 @@
       <c r="E23" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>79</v>
+      <c r="F23" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="G23" t="s">
         <v>79</v>
@@ -2542,7 +2557,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="203" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>171</v>
       </c>
@@ -2553,13 +2568,13 @@
         <v>44561</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E24" t="s">
         <v>79</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="G24" t="s">
         <v>79</v>
@@ -2588,22 +2603,22 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B25" s="1">
         <v>40806</v>
       </c>
       <c r="C25" s="1">
-        <v>40817</v>
+        <v>40807</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>79</v>
+      <c r="F25" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="G25" t="s">
         <v>79</v>
@@ -2632,12 +2647,16 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43831</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44561</v>
+      </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E26" t="s">
         <v>79</v>
@@ -2676,9 +2695,6 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
       <c r="E27" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
bug fix animation, setup val10_xb
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C43803FF-BD2A-4ED0-BF94-EC379E4C6838}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A0300C-49C1-41F2-99D0-97BC754442AE}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11265" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_runs (2)" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="181">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -569,6 +569,12 @@
   </si>
   <si>
     <t>Increased wet &amp; dry slope, increased modelling depth. Also needed to change time period which is being modelled, as Engelstad wave data does not cover the time period after 2019.</t>
+  </si>
+  <si>
+    <t>val10_xb</t>
+  </si>
+  <si>
+    <t>Same as val9_xb, but higher grid resolution in concurrence with larger modelling depth</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1545,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2691,10 +2697,17 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="B27" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43466</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
       <c r="E27" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
added R2% threshold for whether or not there is a storm, and too the convective heat computation as well. also set up for test run
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A0300C-49C1-41F2-99D0-97BC754442AE}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A3BF261-E029-409B-B69F-E81154F06CE2}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11265" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
+    <workbookView xWindow="30855" yWindow="960" windowWidth="21600" windowHeight="11265" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_runs (2)" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="183">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>Same as val9_xb, but higher grid resolution in concurrence with larger modelling depth</t>
+  </si>
+  <si>
+    <t>test7_xb</t>
+  </si>
+  <si>
+    <t>Same as val9_xb, but with new runup2% calculator to use as threshold for when to run xbeach</t>
   </si>
 </sst>
 </file>
@@ -1544,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D62850-41A0-483E-B58F-AB9686CF6265}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="A28:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2741,12 +2747,16 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="B28" s="1">
+        <v>40806</v>
+      </c>
+      <c r="C28" s="1">
+        <v>40817</v>
+      </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="E28" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
setup final validation run
to be done after calibration
</commit_message>
<xml_diff>
--- a/runs/overview_runs.xlsx
+++ b/runs/overview_runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/kevin_debruijn_deltares_nl/Documents/Documents/GitHub/thermo-morphological-model/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DC92870-D100-45AD-B16E-AA3A4D3AF543}"/>
+  <xr:revisionPtr revIDLastSave="298" documentId="8_{908CDBBE-D5FF-437E-999C-B60338ED9F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0F83606-DF1E-47D9-8DF6-347E17A4A120}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{A1C3D725-75B5-40E1-AC6A-8CD997986826}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_runs (2)" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="263">
   <si>
     <t>run_id;t_start;t_end;description;;;;;;;;;;</t>
   </si>
@@ -825,6 +825,15 @@
   </si>
   <si>
     <t>Same as val_gt17, but with varying values for k_soil_frozen [0.7, 1.7, 2.7], k_soil_unfrozen [0.6, 1.05, 1.5], nb [0.45, 0.55, 0.65], flux_factor [1, 0.8, 0.7], and with a thermal subgrid timestep of 36 seconds</t>
+  </si>
+  <si>
+    <t>val_gt24</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Same parameter settings as the best run from cal_gt1 - cal_gt81, which is run … . The following parameter settings are used: k_soil_frozen [...], k_soil_unfrozen [...], nb [...], flux_factor [...], and with a thermal subgrid timestep of 36 seconds. Furthermore, the simulation is now done for 2011, and again repeated 10 times.</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D62850-41A0-483E-B58F-AB9686CF6265}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
@@ -4426,11 +4435,21 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+    <row r="58" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="1">
+        <v>40544</v>
+      </c>
+      <c r="D58" s="1">
+        <v>40909</v>
+      </c>
       <c r="E58" s="2" t="s">
-        <v>77</v>
+        <v>262</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>77</v>

</xml_diff>